<commit_message>
add excel for results in certificate format
</commit_message>
<xml_diff>
--- a/media/comp_data_2018.xlsx
+++ b/media/comp_data_2018.xlsx
@@ -5,14 +5,20 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DL/tmv_src/asogt/media/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DL/tmv_src/heroku/asogt/media/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="competitions" sheetId="26" r:id="rId1"/>
+    <sheet name="certificate-competitions" sheetId="27" r:id="rId2"/>
+    <sheet name="certificate-common_fields" sheetId="30" r:id="rId3"/>
+    <sheet name="certificate-cols" sheetId="32" r:id="rId4"/>
+    <sheet name="certificate-grades" sheetId="28" r:id="rId5"/>
+    <sheet name="certificate-gender" sheetId="29" r:id="rId6"/>
+    <sheet name="certificate-states" sheetId="31" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">competitions!$A$1:$G$1</definedName>
@@ -33,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="210">
   <si>
     <t>PP</t>
   </si>
@@ -330,13 +336,346 @@
   </si>
   <si>
     <t>SpYImS</t>
+  </si>
+  <si>
+    <t>ghyh;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ftpij kddg; </t>
+  </si>
+  <si>
+    <t>Palar</t>
+  </si>
+  <si>
+    <t>Poetry</t>
+  </si>
+  <si>
+    <t>Muk;g</t>
+  </si>
+  <si>
+    <t>Beginner</t>
+  </si>
+  <si>
+    <t>tha;nkhopj; njhlh;ghw;wy;</t>
+  </si>
+  <si>
+    <t>Verbal Communication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fPo;g; </t>
+  </si>
+  <si>
+    <t>Lower</t>
+  </si>
+  <si>
+    <t>kj;jpa</t>
+  </si>
+  <si>
+    <t>Intermediate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vOj;jwpTg; </t>
+  </si>
+  <si>
+    <t>Writing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ngr;Rg;  </t>
+  </si>
+  <si>
+    <t>Speech</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nkw; </t>
+  </si>
+  <si>
+    <t>Senior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mbg;gil vOj;jwpTg; </t>
+  </si>
+  <si>
+    <t>Basic Writing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mjpNkw; </t>
+  </si>
+  <si>
+    <t>Advanced Senior</t>
+  </si>
+  <si>
+    <t>,isQu;</t>
+  </si>
+  <si>
+    <t>Youth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tpNrl vOj;jwpTg; </t>
+  </si>
+  <si>
+    <t>Special Writing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jpUf;Fws; - tpNrl ftpij kddg;  </t>
+  </si>
+  <si>
+    <t>Special Poetry (Thirukkural)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tpNrl jdp ebg;Gg;  </t>
+  </si>
+  <si>
+    <t>Special Acting</t>
+  </si>
+  <si>
+    <t>tpNrl mbg;gilj; jkpohu;t vOj;jwpTj;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nghl;bapy; </t>
+  </si>
+  <si>
+    <t>jpUf;Fws; - tpNrl ftpij kddg;</t>
+  </si>
+  <si>
+    <t>Nju;tpy;</t>
+  </si>
+  <si>
+    <t>tpthjg;</t>
+  </si>
+  <si>
+    <t>tpdhb tpdhg;</t>
+  </si>
+  <si>
+    <t>tpNrl mbg;gil jkpohu;t vOj;jwpTj;</t>
+  </si>
+  <si>
+    <t>Mj;jpR+b - tpNrl ftpij kddg;</t>
+  </si>
+  <si>
+    <t>Special Basic Writing</t>
+  </si>
+  <si>
+    <t>Junior</t>
+  </si>
+  <si>
+    <t>,ilepiy</t>
+  </si>
+  <si>
+    <t>Special Poetry (Aathisoodi)</t>
+  </si>
+  <si>
+    <t>Special Impromptu Speech</t>
+  </si>
+  <si>
+    <t>tpNrl Kd;Ndw;ghlw;w Ngr;Rg;</t>
+  </si>
+  <si>
+    <t>Debate </t>
+  </si>
+  <si>
+    <t>Quiz</t>
+  </si>
+  <si>
+    <t>Kjyhk; ghpR (</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>epiy)</t>
+  </si>
+  <si>
+    <t>First Prize (Grade A)</t>
+  </si>
+  <si>
+    <t>,uz;lhk; ghpR (</t>
+  </si>
+  <si>
+    <t>Second Prize (Grade A)</t>
+  </si>
+  <si>
+    <t>%d;whk; ghpR (</t>
+  </si>
+  <si>
+    <t>Third Prize (Grade A)</t>
+  </si>
+  <si>
+    <t>Grade A</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>epiy</t>
+  </si>
+  <si>
+    <t>Grade B</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Grade C</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>nry;tp;</t>
+  </si>
+  <si>
+    <t>Miss</t>
+  </si>
+  <si>
+    <t>nry;td;</t>
+  </si>
+  <si>
+    <t>Mas.</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>gphptpw;fhd</t>
+  </si>
+  <si>
+    <t>T7</t>
+  </si>
+  <si>
+    <t>T8</t>
+  </si>
+  <si>
+    <t>T8B</t>
+  </si>
+  <si>
+    <t>T9</t>
+  </si>
+  <si>
+    <t>T9A</t>
+  </si>
+  <si>
+    <t>T10</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>E7</t>
+  </si>
+  <si>
+    <t>E8</t>
+  </si>
+  <si>
+    <t>E9</t>
+  </si>
+  <si>
+    <t>E10</t>
+  </si>
+  <si>
+    <t>competition</t>
+  </si>
+  <si>
+    <t>E12</t>
+  </si>
+  <si>
+    <t>Australia.</t>
+  </si>
+  <si>
+    <t>division</t>
+  </si>
+  <si>
+    <t>T6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">khepy epiyapy; eilngw;w  </t>
+  </si>
+  <si>
+    <t>ngw;wikf;fhf toq;fg;gl;lJ.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is to certify that </t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>awarded</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in the </t>
+  </si>
+  <si>
+    <t>QLD</t>
+  </si>
+  <si>
+    <t>NSW</t>
+  </si>
+  <si>
+    <t>gpwp];Ngd;&gt; Fapd;];yhe;J</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>E11</t>
+  </si>
+  <si>
+    <t>in QLD,</t>
+  </si>
+  <si>
+    <t>in NSW,</t>
+  </si>
+  <si>
+    <t>rpl;dp&gt; epA+ rTj; Nty;];</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>COLS</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>First Prize</t>
+  </si>
+  <si>
+    <t>Second Prize</t>
+  </si>
+  <si>
+    <t>Third Prize</t>
+  </si>
+  <si>
+    <t>details</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -420,6 +759,46 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Bamini Plain"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Bamini"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -441,7 +820,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -552,11 +931,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -668,9 +1063,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -972,8 +1388,8 @@
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="23.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1863,4 +2279,1389 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.83203125" style="40"/>
+    <col min="4" max="4" width="43.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33" style="40" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="40"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="48" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="47"/>
+      <c r="B1" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" s="48" t="s">
+        <v>165</v>
+      </c>
+      <c r="D1" s="48" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="F1" s="48" t="s">
+        <v>176</v>
+      </c>
+      <c r="G1" s="48" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D2" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D3" s="43" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="L3"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3"/>
+      <c r="P3"/>
+    </row>
+    <row r="4" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D4" s="43" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="L4"/>
+    </row>
+    <row r="5" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D5" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="L5"/>
+      <c r="M5" s="42"/>
+      <c r="N5" s="42"/>
+      <c r="O5"/>
+      <c r="P5"/>
+    </row>
+    <row r="6" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="43" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D6" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="E6" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="L6"/>
+    </row>
+    <row r="7" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D7" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="E7" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="L7"/>
+    </row>
+    <row r="8" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D8" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="E8" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="L8"/>
+    </row>
+    <row r="9" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="C9" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D9" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="E9" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="L9"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="42"/>
+      <c r="O9"/>
+      <c r="P9"/>
+    </row>
+    <row r="10" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="C10" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D10" s="43" t="s">
+        <v>142</v>
+      </c>
+      <c r="E10" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="G10" s="41" t="s">
+        <v>141</v>
+      </c>
+      <c r="L10"/>
+    </row>
+    <row r="11" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D11" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="E11" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="G11" s="41" t="s">
+        <v>143</v>
+      </c>
+      <c r="L11"/>
+      <c r="M11" s="42"/>
+      <c r="N11" s="42"/>
+      <c r="O11"/>
+      <c r="P11"/>
+    </row>
+    <row r="12" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="C12" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D12" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="E12" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="G12" s="41" t="s">
+        <v>144</v>
+      </c>
+      <c r="L12"/>
+    </row>
+    <row r="13" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="C13" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D13" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="E13" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="L13"/>
+    </row>
+    <row r="14" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D14" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="L14"/>
+    </row>
+    <row r="15" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="43" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D15" s="43" t="s">
+        <v>113</v>
+      </c>
+      <c r="E15" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="L15"/>
+    </row>
+    <row r="16" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="C16" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D16" s="43" t="s">
+        <v>113</v>
+      </c>
+      <c r="E16" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="L16"/>
+    </row>
+    <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D17" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="E17" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="L17"/>
+    </row>
+    <row r="18" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D18" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="L18"/>
+    </row>
+    <row r="19" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="43" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D19" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="E19" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="L19"/>
+    </row>
+    <row r="20" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="C20" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D20" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="L20"/>
+    </row>
+    <row r="21" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D21" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="L21"/>
+    </row>
+    <row r="22" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D22" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="E22" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="L22"/>
+    </row>
+    <row r="23" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D23" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="E23" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="L23"/>
+    </row>
+    <row r="24" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="43" t="s">
+        <v>115</v>
+      </c>
+      <c r="C24" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D24" s="43" t="s">
+        <v>111</v>
+      </c>
+      <c r="E24" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="L24"/>
+    </row>
+    <row r="25" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D25" s="43" t="s">
+        <v>111</v>
+      </c>
+      <c r="E25" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="L25"/>
+    </row>
+    <row r="26" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D26" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="E26" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="L26"/>
+    </row>
+    <row r="27" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="43" t="s">
+        <v>115</v>
+      </c>
+      <c r="C27" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D27" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="E27" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="C28" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D28" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="E28" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="43" t="s">
+        <v>115</v>
+      </c>
+      <c r="C29" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D29" s="43" t="s">
+        <v>135</v>
+      </c>
+      <c r="E29" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D30" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="E30" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="C31" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D31" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="E31" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="C32" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D32" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="E32" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G32" s="41" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="41"/>
+      <c r="B33" s="41"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="41"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="41"/>
+      <c r="B34" s="41"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="41"/>
+      <c r="F34" s="41"/>
+      <c r="G34" s="41"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="41"/>
+      <c r="B35" s="41"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="41"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="41"/>
+      <c r="G35" s="41"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="41"/>
+      <c r="B36" s="41"/>
+      <c r="C36" s="41"/>
+      <c r="D36" s="41"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
+      <c r="G36" s="41"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="41"/>
+      <c r="B37" s="41"/>
+      <c r="C37" s="41"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
+      <c r="G37" s="41"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="41"/>
+      <c r="B38" s="41"/>
+      <c r="C38" s="41"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="41"/>
+      <c r="G38" s="41"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="41"/>
+      <c r="B39" s="41"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="41"/>
+      <c r="E39" s="41"/>
+      <c r="F39" s="41"/>
+      <c r="G39" s="41"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="41"/>
+      <c r="B40" s="41"/>
+      <c r="C40" s="41"/>
+      <c r="D40" s="41"/>
+      <c r="E40" s="41"/>
+      <c r="F40" s="41"/>
+      <c r="G40" s="41"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="41" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="41" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="41" t="s">
+        <v>172</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="B5" s="49" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="B6" s="49" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="B7" s="49" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="41" t="s">
+        <v>177</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="41" t="s">
+        <v>179</v>
+      </c>
+      <c r="B9" s="49" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="41" t="s">
+        <v>181</v>
+      </c>
+      <c r="B10" s="49" t="s">
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="50" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>181</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="41" t="s">
+        <v>206</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2" s="41" t="s">
+        <v>146</v>
+      </c>
+      <c r="D2" s="45" t="s">
+        <v>147</v>
+      </c>
+      <c r="E2" s="46" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="41" t="s">
+        <v>207</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>146</v>
+      </c>
+      <c r="D3" s="45" t="s">
+        <v>147</v>
+      </c>
+      <c r="E3" s="46" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="41" t="s">
+        <v>208</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" s="41" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="45" t="s">
+        <v>147</v>
+      </c>
+      <c r="E4" s="46" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="41" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>146</v>
+      </c>
+      <c r="D5" s="45" t="s">
+        <v>155</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="41" t="s">
+        <v>156</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>154</v>
+      </c>
+      <c r="C6" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="D6" s="45" t="s">
+        <v>155</v>
+      </c>
+      <c r="E6" s="41" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="41" t="s">
+        <v>158</v>
+      </c>
+      <c r="B7" s="45" t="s">
+        <v>154</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="D7" s="45" t="s">
+        <v>155</v>
+      </c>
+      <c r="E7" s="41" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="41"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="41"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="41"/>
+      <c r="B1" s="41" t="s">
+        <v>173</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>201</v>
+      </c>
+      <c r="D1" s="41"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="D2" s="41"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="41" t="s">
+        <v>205</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>163</v>
+      </c>
+      <c r="D3" s="41"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="41"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="41"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix unicode bugs and add participate grade
</commit_message>
<xml_diff>
--- a/media/comp_data_2018.xlsx
+++ b/media/comp_data_2018.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="competitions" sheetId="26" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="219">
   <si>
     <t>PP</t>
   </si>
@@ -669,6 +669,33 @@
   </si>
   <si>
     <t>details</t>
+  </si>
+  <si>
+    <t>STD ID</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>ENG</t>
+  </si>
+  <si>
+    <t>TAMIL</t>
+  </si>
+  <si>
+    <t>FORMAT</t>
+  </si>
+  <si>
+    <t>Participated</t>
+  </si>
+  <si>
+    <t>jifik ngw;wikf;fhf toq;fg;gl;lJ.</t>
+  </si>
+  <si>
+    <t>participated</t>
+  </si>
+  <si>
+    <t>gq;F gw;wpaikf;fhf toq;fg;gl;lJ.</t>
   </si>
 </sst>
 </file>
@@ -3153,7 +3180,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
@@ -3187,57 +3214,41 @@
     </row>
     <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="s">
-        <v>172</v>
-      </c>
-      <c r="B4" s="44" t="s">
-        <v>186</v>
+        <v>174</v>
+      </c>
+      <c r="B4" s="49" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="41" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
       <c r="B5" s="49" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="41" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="B6" s="49" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="41" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="41" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="B8" s="49" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="41" t="s">
-        <v>179</v>
-      </c>
-      <c r="B9" s="49" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="41" t="s">
-        <v>181</v>
-      </c>
-      <c r="B10" s="49" t="s">
         <v>182</v>
       </c>
     </row>
@@ -3248,137 +3259,228 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="50" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" s="50" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B8" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B9" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="B10" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="B11" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="B12" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="B13" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="B14" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="B15" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="B16" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="B17" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="B18" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="B19" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="B20" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="B21" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="B22" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="B23" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="B24" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="B25" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="B26" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>181</v>
+      </c>
+      <c r="B27" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -3388,20 +3490,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.83203125" style="40" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.83203125" style="41" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>169</v>
       </c>
@@ -3411,11 +3515,17 @@
       <c r="D1" t="s">
         <v>171</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="G1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="s">
         <v>206</v>
       </c>
@@ -3428,11 +3538,17 @@
       <c r="D2" s="45" t="s">
         <v>147</v>
       </c>
-      <c r="E2" s="46" t="s">
+      <c r="E2" s="44" t="s">
+        <v>186</v>
+      </c>
+      <c r="F2" s="46" t="s">
+        <v>189</v>
+      </c>
+      <c r="G2" s="46" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="s">
         <v>207</v>
       </c>
@@ -3445,11 +3561,17 @@
       <c r="D3" s="45" t="s">
         <v>147</v>
       </c>
-      <c r="E3" s="46" t="s">
+      <c r="E3" s="44" t="s">
+        <v>186</v>
+      </c>
+      <c r="F3" s="46" t="s">
+        <v>189</v>
+      </c>
+      <c r="G3" s="46" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="s">
         <v>208</v>
       </c>
@@ -3462,11 +3584,17 @@
       <c r="D4" s="45" t="s">
         <v>147</v>
       </c>
-      <c r="E4" s="46" t="s">
+      <c r="E4" s="44" t="s">
+        <v>186</v>
+      </c>
+      <c r="F4" s="46" t="s">
+        <v>189</v>
+      </c>
+      <c r="G4" s="46" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="41" t="s">
         <v>153</v>
       </c>
@@ -3479,11 +3607,17 @@
       <c r="D5" s="45" t="s">
         <v>155</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="44" t="s">
+        <v>216</v>
+      </c>
+      <c r="F5" s="46" t="s">
+        <v>189</v>
+      </c>
+      <c r="G5" s="41" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="41" t="s">
         <v>156</v>
       </c>
@@ -3496,11 +3630,17 @@
       <c r="D6" s="45" t="s">
         <v>155</v>
       </c>
-      <c r="E6" s="41" t="s">
+      <c r="E6" s="44" t="s">
+        <v>216</v>
+      </c>
+      <c r="F6" s="46" t="s">
+        <v>189</v>
+      </c>
+      <c r="G6" s="41" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="41" t="s">
         <v>158</v>
       </c>
@@ -3513,23 +3653,56 @@
       <c r="D7" s="45" t="s">
         <v>155</v>
       </c>
-      <c r="E7" s="41" t="s">
+      <c r="E7" s="44" t="s">
+        <v>216</v>
+      </c>
+      <c r="F7" s="46" t="s">
+        <v>189</v>
+      </c>
+      <c r="G7" s="41" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="41"/>
-      <c r="B8" s="41"/>
+    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="41" t="s">
+        <v>215</v>
+      </c>
+      <c r="B8" s="45"/>
       <c r="C8" s="41"/>
       <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E8" s="44" t="s">
+        <v>218</v>
+      </c>
+      <c r="F8" s="46" t="s">
+        <v>217</v>
+      </c>
+      <c r="G8" s="41"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="41"/>
       <c r="B9" s="41"/>
       <c r="C9" s="41"/>
       <c r="D9" s="41"/>
       <c r="E9" s="41"/>
+      <c r="G9" s="41"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E10" s="41"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E11" s="41"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E12" s="41"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E13" s="41"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E14" s="41"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E15" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3540,7 +3713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -3602,7 +3775,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fix bugs for other states
</commit_message>
<xml_diff>
--- a/media/comp_data_2018.xlsx
+++ b/media/comp_data_2018.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="competitions" sheetId="26" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="240">
   <si>
     <t>PP</t>
   </si>
@@ -702,6 +702,63 @@
   </si>
   <si>
     <t>tpNrl jdp ebg;Gg;</t>
+  </si>
+  <si>
+    <t>VIC</t>
+  </si>
+  <si>
+    <t>in VIC,</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>ACT</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>NZW</t>
+  </si>
+  <si>
+    <t>NZH</t>
+  </si>
+  <si>
+    <t>in SA,</t>
+  </si>
+  <si>
+    <t>in ACT,</t>
+  </si>
+  <si>
+    <t>in WA,</t>
+  </si>
+  <si>
+    <t>in NZW</t>
+  </si>
+  <si>
+    <t>in NZH</t>
+  </si>
+  <si>
+    <t>nky;Ngu;d;&gt; tpf;Nuhupah</t>
+  </si>
+  <si>
+    <t>mbiyl;&gt; rTj; M];jpNuypah</t>
+  </si>
+  <si>
+    <t>fd;nguh&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ngu;j; </t>
+  </si>
+  <si>
+    <t>ntypq;ld;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`hkpy;ld; </t>
+  </si>
+  <si>
+    <t>New Zealand.</t>
   </si>
 </sst>
 </file>
@@ -2318,7 +2375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -3186,10 +3243,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3248,14 +3305,6 @@
       </c>
       <c r="B7" s="49" t="s">
         <v>177</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="41" t="s">
-        <v>178</v>
-      </c>
-      <c r="B8" s="49" t="s">
-        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -3778,18 +3827,19 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
         <v>192</v>
@@ -3797,8 +3847,11 @@
       <c r="C1" s="3" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>189</v>
       </c>
@@ -3808,8 +3861,11 @@
       <c r="C2" s="3" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="D2" s="49" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>190</v>
       </c>
@@ -3819,26 +3875,100 @@
       <c r="C3" s="3" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="D3" s="49" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>233</v>
+      </c>
+      <c r="C4" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="D4" s="49" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>234</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>228</v>
+      </c>
+      <c r="D5" s="49" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="41" t="s">
+        <v>224</v>
+      </c>
+      <c r="B6" s="44" t="s">
+        <v>235</v>
+      </c>
+      <c r="C6" s="41" t="s">
+        <v>229</v>
+      </c>
+      <c r="D6" s="49" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="41" t="s">
+        <v>225</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>236</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>230</v>
+      </c>
+      <c r="D7" s="49" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="41" t="s">
+        <v>226</v>
+      </c>
+      <c r="B8" s="44" t="s">
+        <v>237</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>231</v>
+      </c>
+      <c r="D8" s="49" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="41" t="s">
+        <v>227</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>238</v>
+      </c>
+      <c r="C9" s="41" t="s">
+        <v>232</v>
+      </c>
+      <c r="D9" s="49" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="41"/>
+      <c r="B10" s="44"/>
+    </row>
+    <row r="24" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G24" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix for new updates on asogt
</commit_message>
<xml_diff>
--- a/media/comp_data_2018.xlsx
+++ b/media/comp_data_2018.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="competitions" sheetId="26" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="252">
   <si>
     <t>PP</t>
   </si>
@@ -650,15 +650,6 @@
     <t>Male</t>
   </si>
   <si>
-    <t>First Prize</t>
-  </si>
-  <si>
-    <t>Second Prize</t>
-  </si>
-  <si>
-    <t>Third Prize</t>
-  </si>
-  <si>
     <t>details</t>
   </si>
   <si>
@@ -759,13 +750,58 @@
   </si>
   <si>
     <t>New Zealand.</t>
+  </si>
+  <si>
+    <t>First Prize-Grade A</t>
+  </si>
+  <si>
+    <t>Second Prize-Grade A</t>
+  </si>
+  <si>
+    <t>First Prize-Grade B</t>
+  </si>
+  <si>
+    <t>Second Prize-Grade B</t>
+  </si>
+  <si>
+    <t>Third Prize-Grade C</t>
+  </si>
+  <si>
+    <t>Third Prize-Grade B</t>
+  </si>
+  <si>
+    <t>First Prize-Grade C</t>
+  </si>
+  <si>
+    <t>Second Prize-Grade C</t>
+  </si>
+  <si>
+    <t>First Prize (Grade B)</t>
+  </si>
+  <si>
+    <t>Second Prize (Grade B)</t>
+  </si>
+  <si>
+    <t>Third Prize (Grade B)</t>
+  </si>
+  <si>
+    <t>First Prize (Grade C)</t>
+  </si>
+  <si>
+    <t>Second Prize (Grade C)</t>
+  </si>
+  <si>
+    <t>Third Prize (Grade C)</t>
+  </si>
+  <si>
+    <t>Third Prize-Grade A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -865,12 +901,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
@@ -888,6 +918,29 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Bamini Plain"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <name val="Bamini"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1041,7 +1094,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1164,15 +1217,22 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2390,24 +2450,24 @@
     <col min="8" max="16384" width="10.83203125" style="40"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="48" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="47"/>
-      <c r="B1" s="48" t="s">
+    <row r="1" spans="1:16" s="47" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="46"/>
+      <c r="B1" s="47" t="s">
         <v>161</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="47" t="s">
         <v>162</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="47" t="s">
         <v>164</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="47" t="s">
         <v>165</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="47" t="s">
         <v>173</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="47" t="s">
         <v>175</v>
       </c>
     </row>
@@ -2445,7 +2505,7 @@
         <v>163</v>
       </c>
       <c r="D3" s="43" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E3" s="44" t="s">
         <v>129</v>
@@ -2473,7 +2533,7 @@
         <v>163</v>
       </c>
       <c r="D4" s="43" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E4" s="44" t="s">
         <v>129</v>
@@ -2525,7 +2585,7 @@
         <v>163</v>
       </c>
       <c r="D6" s="43" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E6" s="44" t="s">
         <v>129</v>
@@ -2600,7 +2660,7 @@
         <v>128</v>
       </c>
       <c r="E9" s="44" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>136</v>
@@ -2658,7 +2718,7 @@
         <v>122</v>
       </c>
       <c r="G11" s="41" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L11"/>
       <c r="M11" s="42"/>
@@ -3086,7 +3146,7 @@
         <v>133</v>
       </c>
       <c r="E29" s="44" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>116</v>
@@ -3256,7 +3316,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -3279,7 +3339,7 @@
       <c r="A4" s="41" t="s">
         <v>171</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="48" t="s">
         <v>184</v>
       </c>
     </row>
@@ -3287,7 +3347,7 @@
       <c r="A5" s="41" t="s">
         <v>187</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="48" t="s">
         <v>188</v>
       </c>
     </row>
@@ -3295,7 +3355,7 @@
       <c r="A6" s="41" t="s">
         <v>174</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="48" t="s">
         <v>180</v>
       </c>
     </row>
@@ -3303,7 +3363,7 @@
       <c r="A7" s="41" t="s">
         <v>176</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="48" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3323,27 +3383,27 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="49" t="s">
         <v>200</v>
       </c>
-      <c r="B1" s="50" t="s">
-        <v>211</v>
+      <c r="B1" s="49" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -3351,7 +3411,7 @@
         <v>170</v>
       </c>
       <c r="B4" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -3359,7 +3419,7 @@
         <v>197</v>
       </c>
       <c r="B5" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -3367,7 +3427,7 @@
         <v>161</v>
       </c>
       <c r="B6" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -3375,7 +3435,7 @@
         <v>162</v>
       </c>
       <c r="B7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -3383,7 +3443,7 @@
         <v>192</v>
       </c>
       <c r="B8" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -3391,7 +3451,7 @@
         <v>181</v>
       </c>
       <c r="B9" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -3399,7 +3459,7 @@
         <v>164</v>
       </c>
       <c r="B10" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -3407,7 +3467,7 @@
         <v>165</v>
       </c>
       <c r="B11" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -3415,7 +3475,7 @@
         <v>166</v>
       </c>
       <c r="B12" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -3423,7 +3483,7 @@
         <v>167</v>
       </c>
       <c r="B13" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -3431,7 +3491,7 @@
         <v>168</v>
       </c>
       <c r="B14" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -3439,7 +3499,7 @@
         <v>169</v>
       </c>
       <c r="B15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -3447,7 +3507,7 @@
         <v>171</v>
       </c>
       <c r="B16" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -3455,7 +3515,7 @@
         <v>198</v>
       </c>
       <c r="B17" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -3463,7 +3523,7 @@
         <v>199</v>
       </c>
       <c r="B18" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -3471,7 +3531,7 @@
         <v>185</v>
       </c>
       <c r="B19" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -3479,7 +3539,7 @@
         <v>172</v>
       </c>
       <c r="B20" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -3487,7 +3547,7 @@
         <v>187</v>
       </c>
       <c r="B21" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -3495,7 +3555,7 @@
         <v>173</v>
       </c>
       <c r="B22" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -3503,7 +3563,7 @@
         <v>174</v>
       </c>
       <c r="B23" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -3511,7 +3571,7 @@
         <v>175</v>
       </c>
       <c r="B24" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -3519,7 +3579,7 @@
         <v>176</v>
       </c>
       <c r="B25" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -3527,7 +3587,7 @@
         <v>193</v>
       </c>
       <c r="B26" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -3535,7 +3595,7 @@
         <v>178</v>
       </c>
       <c r="B27" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -3545,219 +3605,359 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" customWidth="1"/>
-    <col min="5" max="5" width="34.83203125" style="40" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.1640625" style="40" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34.83203125" style="41" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="50"/>
+      <c r="B1" s="50" t="s">
         <v>166</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="50" t="s">
         <v>167</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="50" t="s">
         <v>168</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="51" t="s">
         <v>169</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="52" t="s">
         <v>185</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="50" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="41" t="s">
-        <v>203</v>
-      </c>
-      <c r="B2" s="45" t="s">
+    <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="52" t="s">
+        <v>237</v>
+      </c>
+      <c r="B2" s="53" t="s">
         <v>142</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="52" t="s">
         <v>143</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="53" t="s">
         <v>144</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="54" t="s">
         <v>183</v>
       </c>
-      <c r="F2" s="46" t="s">
+      <c r="F2" s="55" t="s">
         <v>186</v>
       </c>
-      <c r="G2" s="46" t="s">
+      <c r="G2" s="55" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="41" t="s">
-        <v>204</v>
-      </c>
-      <c r="B3" s="45" t="s">
+    <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="52" t="s">
+        <v>238</v>
+      </c>
+      <c r="B3" s="53" t="s">
         <v>146</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="52" t="s">
         <v>143</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="53" t="s">
         <v>144</v>
       </c>
-      <c r="E3" s="44" t="s">
+      <c r="E3" s="54" t="s">
         <v>183</v>
       </c>
-      <c r="F3" s="46" t="s">
+      <c r="F3" s="55" t="s">
         <v>186</v>
       </c>
-      <c r="G3" s="46" t="s">
+      <c r="G3" s="55" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="41" t="s">
-        <v>205</v>
-      </c>
-      <c r="B4" s="45" t="s">
+    <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="52" t="s">
+        <v>251</v>
+      </c>
+      <c r="B4" s="53" t="s">
         <v>148</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="52" t="s">
         <v>143</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="53" t="s">
         <v>144</v>
       </c>
-      <c r="E4" s="44" t="s">
+      <c r="E4" s="54" t="s">
         <v>183</v>
       </c>
-      <c r="F4" s="46" t="s">
+      <c r="F4" s="55" t="s">
         <v>186</v>
       </c>
-      <c r="G4" s="46" t="s">
+      <c r="G4" s="55" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="41" t="s">
+    <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="52" t="s">
+        <v>239</v>
+      </c>
+      <c r="B5" s="53" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" s="52" t="s">
+        <v>154</v>
+      </c>
+      <c r="D5" s="53" t="s">
+        <v>144</v>
+      </c>
+      <c r="E5" s="54" t="s">
+        <v>183</v>
+      </c>
+      <c r="F5" s="55" t="s">
+        <v>186</v>
+      </c>
+      <c r="G5" s="55" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A6" s="52" t="s">
+        <v>240</v>
+      </c>
+      <c r="B6" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" s="52" t="s">
+        <v>154</v>
+      </c>
+      <c r="D6" s="53" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6" s="54" t="s">
+        <v>183</v>
+      </c>
+      <c r="F6" s="55" t="s">
+        <v>186</v>
+      </c>
+      <c r="G6" s="55" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="52" t="s">
+        <v>242</v>
+      </c>
+      <c r="B7" s="53" t="s">
+        <v>148</v>
+      </c>
+      <c r="C7" s="52" t="s">
+        <v>154</v>
+      </c>
+      <c r="D7" s="53" t="s">
+        <v>144</v>
+      </c>
+      <c r="E7" s="54" t="s">
+        <v>183</v>
+      </c>
+      <c r="F7" s="55" t="s">
+        <v>186</v>
+      </c>
+      <c r="G7" s="55" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A8" s="52" t="s">
+        <v>243</v>
+      </c>
+      <c r="B8" s="53" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" s="53" t="s">
+        <v>144</v>
+      </c>
+      <c r="E8" s="54" t="s">
+        <v>183</v>
+      </c>
+      <c r="F8" s="55" t="s">
+        <v>186</v>
+      </c>
+      <c r="G8" s="55" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A9" s="52" t="s">
+        <v>244</v>
+      </c>
+      <c r="B9" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="C9" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="D9" s="53" t="s">
+        <v>144</v>
+      </c>
+      <c r="E9" s="54" t="s">
+        <v>183</v>
+      </c>
+      <c r="F9" s="55" t="s">
+        <v>186</v>
+      </c>
+      <c r="G9" s="55" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="52" t="s">
+        <v>241</v>
+      </c>
+      <c r="B10" s="53" t="s">
+        <v>148</v>
+      </c>
+      <c r="C10" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="D10" s="53" t="s">
+        <v>144</v>
+      </c>
+      <c r="E10" s="54" t="s">
+        <v>183</v>
+      </c>
+      <c r="F10" s="55" t="s">
+        <v>186</v>
+      </c>
+      <c r="G10" s="55" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="52" t="s">
         <v>150</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B11" s="53" t="s">
         <v>151</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C11" s="52" t="s">
         <v>143</v>
       </c>
-      <c r="D5" s="45" t="s">
+      <c r="D11" s="53" t="s">
         <v>152</v>
       </c>
-      <c r="E5" s="44" t="s">
-        <v>213</v>
-      </c>
-      <c r="F5" s="46" t="s">
+      <c r="E11" s="54" t="s">
+        <v>210</v>
+      </c>
+      <c r="F11" s="55" t="s">
         <v>186</v>
       </c>
-      <c r="G5" s="41" t="s">
+      <c r="G11" s="55" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="41" t="s">
+    <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="52" t="s">
         <v>153</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B12" s="53" t="s">
         <v>151</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C12" s="52" t="s">
         <v>154</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D12" s="53" t="s">
         <v>152</v>
       </c>
-      <c r="E6" s="44" t="s">
-        <v>213</v>
-      </c>
-      <c r="F6" s="46" t="s">
+      <c r="E12" s="54" t="s">
+        <v>210</v>
+      </c>
+      <c r="F12" s="55" t="s">
         <v>186</v>
       </c>
-      <c r="G6" s="41" t="s">
+      <c r="G12" s="55" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="41" t="s">
+    <row r="13" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A13" s="52" t="s">
         <v>155</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B13" s="53" t="s">
         <v>151</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C13" s="52" t="s">
         <v>156</v>
       </c>
-      <c r="D7" s="45" t="s">
+      <c r="D13" s="53" t="s">
         <v>152</v>
       </c>
-      <c r="E7" s="44" t="s">
-        <v>213</v>
-      </c>
-      <c r="F7" s="46" t="s">
+      <c r="E13" s="54" t="s">
+        <v>210</v>
+      </c>
+      <c r="F13" s="55" t="s">
         <v>186</v>
       </c>
-      <c r="G7" s="41" t="s">
+      <c r="G13" s="55" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="41" t="s">
+    <row r="14" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A14" s="52" t="s">
+        <v>209</v>
+      </c>
+      <c r="B14" s="53"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="54" t="s">
         <v>212</v>
       </c>
-      <c r="B8" s="45"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="44" t="s">
-        <v>215</v>
-      </c>
-      <c r="F8" s="46" t="s">
-        <v>214</v>
-      </c>
-      <c r="G8" s="41"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="41"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="G9" s="41"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E10" s="41"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E11" s="41"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E12" s="41"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E13" s="41"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E14" s="41"/>
+      <c r="F14" s="55" t="s">
+        <v>211</v>
+      </c>
+      <c r="G14" s="52"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="41"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
       <c r="E15" s="41"/>
+      <c r="G15" s="41"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E16" s="41"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E17" s="41"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E18" s="41"/>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E19" s="41"/>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E20" s="41"/>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E21" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3829,7 +4029,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -3861,7 +4061,7 @@
       <c r="C2" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="48" t="s">
         <v>179</v>
       </c>
     </row>
@@ -3875,92 +4075,92 @@
       <c r="C3" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="48" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B4" s="44" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C4" s="41" t="s">
-        <v>222</v>
-      </c>
-      <c r="D4" s="49" t="s">
+        <v>219</v>
+      </c>
+      <c r="D4" s="48" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="41" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C5" s="41" t="s">
-        <v>228</v>
-      </c>
-      <c r="D5" s="49" t="s">
+        <v>225</v>
+      </c>
+      <c r="D5" s="48" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="41" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B6" s="44" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C6" s="41" t="s">
-        <v>229</v>
-      </c>
-      <c r="D6" s="49" t="s">
+        <v>226</v>
+      </c>
+      <c r="D6" s="48" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="41" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B7" s="44" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C7" s="41" t="s">
-        <v>230</v>
-      </c>
-      <c r="D7" s="49" t="s">
+        <v>227</v>
+      </c>
+      <c r="D7" s="48" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="41" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B8" s="44" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C8" s="41" t="s">
-        <v>231</v>
-      </c>
-      <c r="D8" s="49" t="s">
-        <v>239</v>
+        <v>228</v>
+      </c>
+      <c r="D8" s="48" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="41" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B9" s="44" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C9" s="41" t="s">
-        <v>232</v>
-      </c>
-      <c r="D9" s="49" t="s">
-        <v>239</v>
+        <v>229</v>
+      </c>
+      <c r="D9" s="48" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
clean up things and enable other states
</commit_message>
<xml_diff>
--- a/media/comp_data_2018.xlsx
+++ b/media/comp_data_2018.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="competitions" sheetId="26" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="253">
   <si>
     <t>PP</t>
   </si>
@@ -209,9 +209,6 @@
     <t>விசேட தனி நடிப்புப் போட்டி - மேற் பிரிவு</t>
   </si>
   <si>
-    <t>விசேட முன்னேற்பாடற்ற பேச்சுப் போட்டி - அதிஇளைஞர் பிரிவு</t>
-  </si>
-  <si>
     <t>AdSQ</t>
   </si>
   <si>
@@ -719,9 +716,6 @@
     <t>in SA,</t>
   </si>
   <si>
-    <t>in ACT,</t>
-  </si>
-  <si>
     <t>in WA,</t>
   </si>
   <si>
@@ -731,18 +725,6 @@
     <t>in NZH</t>
   </si>
   <si>
-    <t>nky;Ngu;d;&gt; tpf;Nuhupah</t>
-  </si>
-  <si>
-    <t>mbiyl;&gt; rTj; M];jpNuypah</t>
-  </si>
-  <si>
-    <t>fd;nguh&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ngu;j; </t>
-  </si>
-  <si>
     <t>ntypq;ld;</t>
   </si>
   <si>
@@ -795,6 +777,27 @@
   </si>
   <si>
     <t>Third Prize-Grade A</t>
+  </si>
+  <si>
+    <t>nky;Ngd;&gt; tpf;Nuhupah</t>
+  </si>
+  <si>
+    <t>in Canberra,</t>
+  </si>
+  <si>
+    <t>njd; mT];jpNuypah</t>
+  </si>
+  <si>
+    <t>fd;guhtpy;</t>
+  </si>
+  <si>
+    <t>Nkw;F mT];jpNuypah</t>
+  </si>
+  <si>
+    <t>SEAT POS</t>
+  </si>
+  <si>
+    <t>விசேட முன்னேற்பாடற்ற பேச்சுப் போட்டி -  அதிஇளைஞர் பிரிவு</t>
   </si>
 </sst>
 </file>
@@ -1094,7 +1097,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1128,24 +1131,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1168,9 +1153,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1233,6 +1215,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1538,46 +1529,46 @@
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="23.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="14.1640625" customWidth="1"/>
-    <col min="3" max="3" width="70" style="31" customWidth="1"/>
+    <col min="3" max="3" width="70" style="24" customWidth="1"/>
     <col min="4" max="4" width="33" style="4" customWidth="1"/>
     <col min="5" max="5" width="27.6640625" style="4" customWidth="1"/>
     <col min="6" max="8" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="28" t="s">
         <v>93</v>
-      </c>
-      <c r="B1" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="C1" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="E1" s="36" t="s">
-        <v>95</v>
-      </c>
-      <c r="F1" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="I1" s="35" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.2">
@@ -1587,14 +1578,14 @@
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2" s="38" t="s">
-        <v>96</v>
+      <c r="D2" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>95</v>
       </c>
       <c r="F2" s="8">
         <v>120</v>
@@ -1613,14 +1604,14 @@
       <c r="B3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F3" s="8">
         <v>180</v>
@@ -1639,14 +1630,14 @@
       <c r="B4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F4" s="8">
         <v>0</v>
@@ -1667,14 +1658,14 @@
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="20" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F5" s="8">
         <v>180</v>
@@ -1694,14 +1685,14 @@
       <c r="B6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="20" t="s">
         <v>55</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F6" s="11">
         <v>300</v>
@@ -1721,14 +1712,14 @@
       <c r="B7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="20" t="s">
         <v>50</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F7" s="11">
         <v>120</v>
@@ -1748,14 +1739,14 @@
       <c r="B8" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="20" t="s">
         <v>54</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F8" s="11">
         <v>180</v>
@@ -1775,12 +1766,12 @@
       <c r="B9" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="20" t="s">
         <v>43</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F9" s="12">
         <v>0</v>
@@ -1795,76 +1786,76 @@
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="13">
+      <c r="A10" s="49">
         <v>11</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="F10" s="16">
+      <c r="B10" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="50" t="s">
+        <v>252</v>
+      </c>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="F10" s="11">
         <v>0</v>
       </c>
-      <c r="G10" s="16">
+      <c r="G10" s="11">
         <v>0</v>
       </c>
-      <c r="H10" s="17">
+      <c r="H10" s="10">
         <v>0</v>
       </c>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="13">
+      <c r="A11" s="49">
         <v>12</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="F11" s="16">
+      <c r="D11" s="51"/>
+      <c r="E11" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="11">
         <v>0</v>
       </c>
-      <c r="G11" s="16">
+      <c r="G11" s="11">
         <v>0</v>
       </c>
-      <c r="H11" s="17">
+      <c r="H11" s="10">
         <v>0</v>
       </c>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="13">
+      <c r="A12" s="49">
         <v>13</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="F12" s="18">
+      <c r="D12" s="51"/>
+      <c r="E12" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" s="12">
         <v>0</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="12">
         <v>0</v>
       </c>
-      <c r="H12" s="17">
+      <c r="H12" s="10">
         <v>0</v>
       </c>
       <c r="I12" s="1"/>
@@ -1876,14 +1867,14 @@
       <c r="B13" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="20" t="s">
         <v>26</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F13" s="8">
         <v>120</v>
@@ -1903,14 +1894,14 @@
       <c r="B14" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F14" s="8">
         <v>130</v>
@@ -1930,14 +1921,14 @@
       <c r="B15" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="20" t="s">
         <v>32</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F15" s="8">
         <v>180</v>
@@ -1957,14 +1948,14 @@
       <c r="B16" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="20" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F16" s="8">
         <v>200</v>
@@ -1984,14 +1975,14 @@
       <c r="B17" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="20" t="s">
         <v>37</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F17" s="8">
         <v>180</v>
@@ -2011,14 +2002,14 @@
       <c r="B18" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="20" t="s">
         <v>39</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F18" s="8">
         <v>300</v>
@@ -2038,14 +2029,14 @@
       <c r="B19" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="20" t="s">
         <v>41</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F19" s="8">
         <v>300</v>
@@ -2065,14 +2056,14 @@
       <c r="B20" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F20" s="8">
         <v>420</v>
@@ -2092,14 +2083,14 @@
       <c r="B21" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F21" s="8">
         <v>420</v>
@@ -2107,7 +2098,7 @@
       <c r="G21" s="8">
         <v>45</v>
       </c>
-      <c r="H21" s="19">
+      <c r="H21" s="13">
         <v>900</v>
       </c>
     </row>
@@ -2118,14 +2109,14 @@
       <c r="B22" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="20" t="s">
         <v>49</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F22" s="12">
         <v>0</v>
@@ -2145,14 +2136,14 @@
       <c r="B23" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="20" t="s">
         <v>47</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F23" s="12">
         <v>0</v>
@@ -2172,14 +2163,14 @@
       <c r="B24" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F24" s="12">
         <v>0</v>
@@ -2199,14 +2190,14 @@
       <c r="B25" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F25" s="8">
         <v>0</v>
@@ -2226,14 +2217,14 @@
       <c r="B26" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F26" s="8">
         <v>0</v>
@@ -2253,14 +2244,14 @@
       <c r="B27" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F27" s="8">
         <v>0</v>
@@ -2280,14 +2271,14 @@
       <c r="B28" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="26" t="s">
+      <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F28" s="12">
         <v>0</v>
@@ -2307,14 +2298,14 @@
       <c r="B29" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="26" t="s">
+      <c r="C29" s="20" t="s">
         <v>45</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F29" s="12">
         <v>0</v>
@@ -2334,19 +2325,19 @@
       <c r="B30" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="20" t="s">
         <v>51</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F30" s="20">
+        <v>95</v>
+      </c>
+      <c r="F30" s="14">
         <v>120</v>
       </c>
-      <c r="G30" s="20">
+      <c r="G30" s="14">
         <v>60</v>
       </c>
       <c r="H30" s="9">
@@ -2360,19 +2351,19 @@
       <c r="B31" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C31" s="26" t="s">
+      <c r="C31" s="20" t="s">
         <v>52</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F31" s="20">
+        <v>95</v>
+      </c>
+      <c r="F31" s="14">
         <v>280</v>
       </c>
-      <c r="G31" s="20">
+      <c r="G31" s="14">
         <v>45</v>
       </c>
       <c r="H31" s="9">
@@ -2380,51 +2371,51 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="21">
+      <c r="A32" s="15">
         <v>33</v>
       </c>
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C32" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="F32" s="24">
+      <c r="D32" s="17"/>
+      <c r="E32" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="F32" s="18">
         <v>0</v>
       </c>
-      <c r="G32" s="24">
+      <c r="G32" s="18">
         <v>0</v>
       </c>
-      <c r="H32" s="25">
+      <c r="H32" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
-      <c r="C33" s="29"/>
+      <c r="C33" s="22"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
-      <c r="C34" s="29"/>
+      <c r="C34" s="22"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="3"/>
-      <c r="C35" s="29"/>
+      <c r="C35" s="22"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
-      <c r="C36" s="29"/>
+      <c r="C36" s="22"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C37" s="30"/>
+      <c r="C37" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2441,860 +2432,860 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.83203125" style="40"/>
-    <col min="4" max="4" width="43.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33" style="40" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="40"/>
+    <col min="1" max="1" width="12.1640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.83203125" style="33"/>
+    <col min="4" max="4" width="43.6640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33" style="33" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="47" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="46"/>
-      <c r="B1" s="47" t="s">
+    <row r="1" spans="1:16" s="40" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="39"/>
+      <c r="B1" s="40" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" s="40" t="s">
         <v>161</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="D1" s="40" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="G1" s="40" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="36" t="s">
         <v>162</v>
       </c>
-      <c r="D1" s="47" t="s">
-        <v>164</v>
-      </c>
-      <c r="E1" s="47" t="s">
-        <v>165</v>
-      </c>
-      <c r="F1" s="47" t="s">
-        <v>173</v>
-      </c>
-      <c r="G1" s="47" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="43" t="s">
+      <c r="D2" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="D2" s="43" t="s">
+      <c r="E2" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>102</v>
-      </c>
     </row>
     <row r="3" spans="1:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>214</v>
+      </c>
+      <c r="E3" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C3" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="D3" s="43" t="s">
-        <v>215</v>
-      </c>
-      <c r="E3" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>110</v>
-      </c>
       <c r="G3" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L3"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
       <c r="O3"/>
       <c r="P3"/>
     </row>
     <row r="4" spans="1:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>215</v>
+      </c>
+      <c r="E4" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C4" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="D4" s="43" t="s">
-        <v>216</v>
-      </c>
-      <c r="E4" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>110</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L4"/>
     </row>
     <row r="5" spans="1:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C5" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="D5" s="43" t="s">
+      <c r="G5" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="E5" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>106</v>
-      </c>
       <c r="L5"/>
-      <c r="M5" s="42"/>
-      <c r="N5" s="42"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
       <c r="O5"/>
       <c r="P5"/>
     </row>
     <row r="6" spans="1:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>216</v>
+      </c>
+      <c r="E6" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C6" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="D6" s="43" t="s">
-        <v>217</v>
-      </c>
-      <c r="E6" s="44" t="s">
+      <c r="G6" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="L6"/>
+    </row>
+    <row r="7" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D7" s="36" t="s">
         <v>129</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="E7" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="L7"/>
+    </row>
+    <row r="8" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="E8" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="L8"/>
+    </row>
+    <row r="9" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D9" s="36" t="s">
         <v>127</v>
       </c>
-      <c r="L6"/>
-    </row>
-    <row r="7" spans="1:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="43" t="s">
-        <v>103</v>
-      </c>
-      <c r="C7" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="D7" s="43" t="s">
-        <v>130</v>
-      </c>
-      <c r="E7" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="L7"/>
-    </row>
-    <row r="8" spans="1:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="43" t="s">
-        <v>109</v>
-      </c>
-      <c r="C8" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="D8" s="43" t="s">
-        <v>130</v>
-      </c>
-      <c r="E8" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="L8"/>
-    </row>
-    <row r="9" spans="1:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="43" t="s">
-        <v>137</v>
-      </c>
-      <c r="C9" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="D9" s="43" t="s">
-        <v>128</v>
-      </c>
-      <c r="E9" s="44" t="s">
-        <v>214</v>
+      <c r="E9" s="37" t="s">
+        <v>213</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L9"/>
-      <c r="M9" s="42"/>
-      <c r="N9" s="42"/>
+      <c r="M9" s="35"/>
+      <c r="N9" s="35"/>
       <c r="O9"/>
       <c r="P9"/>
     </row>
     <row r="10" spans="1:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="39" t="s">
-        <v>98</v>
-      </c>
-      <c r="B10" s="43" t="s">
+      <c r="A10" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D10" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="E10" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C10" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="D10" s="43" t="s">
-        <v>140</v>
-      </c>
-      <c r="E10" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="G10" s="41" t="s">
-        <v>139</v>
+      <c r="G10" s="34" t="s">
+        <v>138</v>
       </c>
       <c r="L10"/>
     </row>
     <row r="11" spans="1:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="43" t="s">
+      <c r="A11" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D11" s="36" t="s">
+        <v>130</v>
+      </c>
+      <c r="E11" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C11" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="D11" s="43" t="s">
-        <v>131</v>
-      </c>
-      <c r="E11" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="G11" s="41" t="s">
-        <v>213</v>
+      <c r="G11" s="34" t="s">
+        <v>212</v>
       </c>
       <c r="L11"/>
-      <c r="M11" s="42"/>
-      <c r="N11" s="42"/>
+      <c r="M11" s="35"/>
+      <c r="N11" s="35"/>
       <c r="O11"/>
       <c r="P11"/>
     </row>
     <row r="12" spans="1:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="B12" s="43" t="s">
+      <c r="A12" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D12" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="E12" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C12" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="D12" s="43" t="s">
+      <c r="G12" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="L12"/>
+    </row>
+    <row r="13" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D13" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="E13" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L13"/>
+    </row>
+    <row r="14" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="E14" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L14"/>
+    </row>
+    <row r="15" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D15" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="E15" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="L15"/>
+    </row>
+    <row r="16" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D16" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="E16" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="L16"/>
+    </row>
+    <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="C17" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D17" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="L17"/>
+    </row>
+    <row r="18" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D18" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="E18" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="L18"/>
+    </row>
+    <row r="19" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D19" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="E19" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="L19"/>
+    </row>
+    <row r="20" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="C20" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D20" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="E20" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="L20"/>
+    </row>
+    <row r="21" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="C21" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D21" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="L21"/>
+    </row>
+    <row r="22" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D22" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="E22" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="L22"/>
+    </row>
+    <row r="23" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D23" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="E23" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="L23"/>
+    </row>
+    <row r="24" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="C24" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D24" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="E24" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="L24"/>
+    </row>
+    <row r="25" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="C25" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D25" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="E25" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="L25"/>
+    </row>
+    <row r="26" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D26" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="E26" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="L26"/>
+    </row>
+    <row r="27" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="C27" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D27" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="E27" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="C28" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D28" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="E28" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="C29" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D29" s="36" t="s">
         <v>132</v>
       </c>
-      <c r="E12" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="G12" s="41" t="s">
-        <v>141</v>
-      </c>
-      <c r="L12"/>
-    </row>
-    <row r="13" spans="1:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="43" t="s">
-        <v>103</v>
-      </c>
-      <c r="C13" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="D13" s="43" t="s">
+      <c r="E29" s="37" t="s">
+        <v>213</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D30" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="E30" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E13" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="L13"/>
-    </row>
-    <row r="14" spans="1:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="C14" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="D14" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="E14" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="L14"/>
-    </row>
-    <row r="15" spans="1:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="43" t="s">
-        <v>115</v>
-      </c>
-      <c r="C15" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="D15" s="43" t="s">
-        <v>113</v>
-      </c>
-      <c r="E15" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="L15"/>
-    </row>
-    <row r="16" spans="1:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="43" t="s">
+      <c r="G30" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="C31" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D31" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="E31" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C16" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="D16" s="43" t="s">
-        <v>113</v>
-      </c>
-      <c r="E16" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="L16"/>
-    </row>
-    <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="C17" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="D17" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="E17" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="L17"/>
-    </row>
-    <row r="18" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="43" t="s">
-        <v>109</v>
-      </c>
-      <c r="C18" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="D18" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="E18" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="L18"/>
-    </row>
-    <row r="19" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="43" t="s">
-        <v>115</v>
-      </c>
-      <c r="C19" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="D19" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="E19" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="L19"/>
-    </row>
-    <row r="20" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="43" t="s">
+      <c r="G31" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="C32" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D32" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="E32" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C20" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="D20" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="E20" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="L20"/>
-    </row>
-    <row r="21" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="C21" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="D21" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="E21" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="L21"/>
-    </row>
-    <row r="22" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="C22" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="D22" s="43" t="s">
-        <v>123</v>
-      </c>
-      <c r="E22" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="L22"/>
-    </row>
-    <row r="23" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="39" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="C23" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="D23" s="43" t="s">
-        <v>123</v>
-      </c>
-      <c r="E23" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="L23"/>
-    </row>
-    <row r="24" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" s="43" t="s">
-        <v>115</v>
-      </c>
-      <c r="C24" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="D24" s="43" t="s">
-        <v>111</v>
-      </c>
-      <c r="E24" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="L24"/>
-    </row>
-    <row r="25" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="C25" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="D25" s="43" t="s">
-        <v>111</v>
-      </c>
-      <c r="E25" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="L25"/>
-    </row>
-    <row r="26" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" s="43" t="s">
-        <v>109</v>
-      </c>
-      <c r="C26" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="D26" s="43" t="s">
-        <v>117</v>
-      </c>
-      <c r="E26" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="L26"/>
-    </row>
-    <row r="27" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="43" t="s">
-        <v>115</v>
-      </c>
-      <c r="C27" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="D27" s="43" t="s">
-        <v>117</v>
-      </c>
-      <c r="E27" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="B28" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="C28" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="D28" s="43" t="s">
-        <v>117</v>
-      </c>
-      <c r="E28" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="43" t="s">
-        <v>115</v>
-      </c>
-      <c r="C29" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="D29" s="43" t="s">
-        <v>133</v>
-      </c>
-      <c r="E29" s="44" t="s">
-        <v>214</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="39" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" s="43" t="s">
-        <v>99</v>
-      </c>
-      <c r="C30" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="D30" s="43" t="s">
-        <v>134</v>
-      </c>
-      <c r="E30" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="B31" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="C31" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="D31" s="43" t="s">
-        <v>125</v>
-      </c>
-      <c r="E31" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="B32" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="C32" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="D32" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="E32" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="G32" s="41" t="s">
-        <v>141</v>
+      <c r="G32" s="34" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="41"/>
-      <c r="B33" s="41"/>
-      <c r="C33" s="41"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="41"/>
+      <c r="A33" s="34"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="41"/>
-      <c r="B34" s="41"/>
-      <c r="C34" s="41"/>
-      <c r="D34" s="41"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="41"/>
-      <c r="G34" s="41"/>
+      <c r="A34" s="34"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="41"/>
-      <c r="B35" s="41"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
-      <c r="G35" s="41"/>
+      <c r="A35" s="34"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="34"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="41"/>
-      <c r="B36" s="41"/>
-      <c r="C36" s="41"/>
-      <c r="D36" s="41"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
-      <c r="G36" s="41"/>
+      <c r="A36" s="34"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="34"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="41"/>
-      <c r="B37" s="41"/>
-      <c r="C37" s="41"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
-      <c r="G37" s="41"/>
+      <c r="A37" s="34"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
+      <c r="G37" s="34"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="41"/>
-      <c r="B38" s="41"/>
-      <c r="C38" s="41"/>
-      <c r="D38" s="41"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="41"/>
-      <c r="G38" s="41"/>
+      <c r="A38" s="34"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
+      <c r="G38" s="34"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="41"/>
-      <c r="B39" s="41"/>
-      <c r="C39" s="41"/>
-      <c r="D39" s="41"/>
-      <c r="E39" s="41"/>
-      <c r="F39" s="41"/>
-      <c r="G39" s="41"/>
+      <c r="A39" s="34"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="34"/>
+      <c r="G39" s="34"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="41"/>
-      <c r="B40" s="41"/>
-      <c r="C40" s="41"/>
-      <c r="D40" s="41"/>
-      <c r="E40" s="41"/>
-      <c r="F40" s="41"/>
-      <c r="G40" s="41"/>
+      <c r="A40" s="34"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="34"/>
+      <c r="G40" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3316,55 +3307,55 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="B2" s="44" t="s">
-        <v>163</v>
-      </c>
     </row>
     <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3" s="37" t="s">
         <v>181</v>
       </c>
-      <c r="B3" s="44" t="s">
-        <v>182</v>
-      </c>
     </row>
     <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="41" t="s">
-        <v>171</v>
-      </c>
-      <c r="B4" s="48" t="s">
-        <v>184</v>
+      <c r="A4" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="B4" s="41" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="34" t="s">
+        <v>186</v>
+      </c>
+      <c r="B5" s="41" t="s">
         <v>187</v>
       </c>
-      <c r="B5" s="48" t="s">
-        <v>188</v>
-      </c>
     </row>
     <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="B6" s="48" t="s">
-        <v>180</v>
+      <c r="A6" s="34" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" s="41" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="B7" s="41" t="s">
         <v>176</v>
-      </c>
-      <c r="B7" s="48" t="s">
-        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -3374,113 +3365,113 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="49" t="s">
-        <v>200</v>
-      </c>
-      <c r="B1" s="49" t="s">
-        <v>208</v>
+      <c r="A1" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B3" t="s">
         <v>205</v>
-      </c>
-      <c r="B3" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>170</v>
+        <v>251</v>
       </c>
       <c r="B4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>197</v>
+        <v>169</v>
       </c>
       <c r="B5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>161</v>
+        <v>196</v>
       </c>
       <c r="B6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>192</v>
+        <v>161</v>
       </c>
       <c r="B8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="B9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>164</v>
+        <v>180</v>
       </c>
       <c r="B10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B13" t="s">
         <v>206</v>
@@ -3488,23 +3479,23 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B14" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B16" t="s">
         <v>206</v>
@@ -3512,90 +3503,98 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>198</v>
+        <v>170</v>
       </c>
       <c r="B17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="B19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
       <c r="B20" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="B21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="B22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B25" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
       <c r="B26" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
       <c r="B27" t="s">
-        <v>206</v>
+        <v>205</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>177</v>
+      </c>
+      <c r="B28" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -3607,8 +3606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3616,348 +3615,348 @@
     <col min="1" max="1" width="24.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" customWidth="1"/>
-    <col min="5" max="5" width="46.1640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.83203125" style="41" customWidth="1"/>
+    <col min="5" max="5" width="46.1640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.83203125" style="34" customWidth="1"/>
     <col min="7" max="7" width="29.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="50"/>
-      <c r="B1" s="50" t="s">
+      <c r="A1" s="43"/>
+      <c r="B1" s="43" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" s="43" t="s">
         <v>166</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="D1" s="43" t="s">
         <v>167</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="E1" s="44" t="s">
         <v>168</v>
       </c>
-      <c r="E1" s="51" t="s">
-        <v>169</v>
-      </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="45" t="s">
+        <v>184</v>
+      </c>
+      <c r="G1" s="43" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="45" t="s">
+        <v>231</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" s="46" t="s">
+        <v>143</v>
+      </c>
+      <c r="E2" s="47" t="s">
+        <v>182</v>
+      </c>
+      <c r="F2" s="48" t="s">
         <v>185</v>
       </c>
-      <c r="G1" s="50" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="52" t="s">
+      <c r="G2" s="48" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="45" t="s">
+        <v>232</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>145</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3" s="46" t="s">
+        <v>143</v>
+      </c>
+      <c r="E3" s="47" t="s">
+        <v>182</v>
+      </c>
+      <c r="F3" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="G3" s="48" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="45" t="s">
+        <v>245</v>
+      </c>
+      <c r="B4" s="46" t="s">
+        <v>147</v>
+      </c>
+      <c r="C4" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" s="46" t="s">
+        <v>143</v>
+      </c>
+      <c r="E4" s="47" t="s">
+        <v>182</v>
+      </c>
+      <c r="F4" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="G4" s="48" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="45" t="s">
+        <v>233</v>
+      </c>
+      <c r="B5" s="46" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="45" t="s">
+        <v>153</v>
+      </c>
+      <c r="D5" s="46" t="s">
+        <v>143</v>
+      </c>
+      <c r="E5" s="47" t="s">
+        <v>182</v>
+      </c>
+      <c r="F5" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="G5" s="48" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A6" s="45" t="s">
+        <v>234</v>
+      </c>
+      <c r="B6" s="46" t="s">
+        <v>145</v>
+      </c>
+      <c r="C6" s="45" t="s">
+        <v>153</v>
+      </c>
+      <c r="D6" s="46" t="s">
+        <v>143</v>
+      </c>
+      <c r="E6" s="47" t="s">
+        <v>182</v>
+      </c>
+      <c r="F6" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="G6" s="48" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="45" t="s">
+        <v>236</v>
+      </c>
+      <c r="B7" s="46" t="s">
+        <v>147</v>
+      </c>
+      <c r="C7" s="45" t="s">
+        <v>153</v>
+      </c>
+      <c r="D7" s="46" t="s">
+        <v>143</v>
+      </c>
+      <c r="E7" s="47" t="s">
+        <v>182</v>
+      </c>
+      <c r="F7" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="G7" s="48" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A8" s="45" t="s">
         <v>237</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B8" s="46" t="s">
+        <v>141</v>
+      </c>
+      <c r="C8" s="45" t="s">
+        <v>155</v>
+      </c>
+      <c r="D8" s="46" t="s">
+        <v>143</v>
+      </c>
+      <c r="E8" s="47" t="s">
+        <v>182</v>
+      </c>
+      <c r="F8" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="G8" s="48" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A9" s="45" t="s">
+        <v>238</v>
+      </c>
+      <c r="B9" s="46" t="s">
+        <v>145</v>
+      </c>
+      <c r="C9" s="45" t="s">
+        <v>155</v>
+      </c>
+      <c r="D9" s="46" t="s">
+        <v>143</v>
+      </c>
+      <c r="E9" s="47" t="s">
+        <v>182</v>
+      </c>
+      <c r="F9" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="G9" s="48" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="45" t="s">
+        <v>235</v>
+      </c>
+      <c r="B10" s="46" t="s">
+        <v>147</v>
+      </c>
+      <c r="C10" s="45" t="s">
+        <v>155</v>
+      </c>
+      <c r="D10" s="46" t="s">
+        <v>143</v>
+      </c>
+      <c r="E10" s="47" t="s">
+        <v>182</v>
+      </c>
+      <c r="F10" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="G10" s="48" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="45" t="s">
+        <v>149</v>
+      </c>
+      <c r="B11" s="46" t="s">
+        <v>150</v>
+      </c>
+      <c r="C11" s="45" t="s">
         <v>142</v>
       </c>
-      <c r="C2" s="52" t="s">
-        <v>143</v>
-      </c>
-      <c r="D2" s="53" t="s">
-        <v>144</v>
-      </c>
-      <c r="E2" s="54" t="s">
-        <v>183</v>
-      </c>
-      <c r="F2" s="55" t="s">
-        <v>186</v>
-      </c>
-      <c r="G2" s="55" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="52" t="s">
-        <v>238</v>
-      </c>
-      <c r="B3" s="53" t="s">
-        <v>146</v>
-      </c>
-      <c r="C3" s="52" t="s">
-        <v>143</v>
-      </c>
-      <c r="D3" s="53" t="s">
-        <v>144</v>
-      </c>
-      <c r="E3" s="54" t="s">
-        <v>183</v>
-      </c>
-      <c r="F3" s="55" t="s">
-        <v>186</v>
-      </c>
-      <c r="G3" s="55" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="52" t="s">
-        <v>251</v>
-      </c>
-      <c r="B4" s="53" t="s">
-        <v>148</v>
-      </c>
-      <c r="C4" s="52" t="s">
-        <v>143</v>
-      </c>
-      <c r="D4" s="53" t="s">
-        <v>144</v>
-      </c>
-      <c r="E4" s="54" t="s">
-        <v>183</v>
-      </c>
-      <c r="F4" s="55" t="s">
-        <v>186</v>
-      </c>
-      <c r="G4" s="55" t="s">
+      <c r="D11" s="46" t="s">
+        <v>151</v>
+      </c>
+      <c r="E11" s="47" t="s">
+        <v>209</v>
+      </c>
+      <c r="F11" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="G11" s="48" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="52" t="s">
-        <v>239</v>
-      </c>
-      <c r="B5" s="53" t="s">
-        <v>142</v>
-      </c>
-      <c r="C5" s="52" t="s">
+    <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="45" t="s">
+        <v>152</v>
+      </c>
+      <c r="B12" s="46" t="s">
+        <v>150</v>
+      </c>
+      <c r="C12" s="45" t="s">
+        <v>153</v>
+      </c>
+      <c r="D12" s="46" t="s">
+        <v>151</v>
+      </c>
+      <c r="E12" s="47" t="s">
+        <v>209</v>
+      </c>
+      <c r="F12" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="G12" s="48" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A13" s="45" t="s">
         <v>154</v>
       </c>
-      <c r="D5" s="53" t="s">
-        <v>144</v>
-      </c>
-      <c r="E5" s="54" t="s">
-        <v>183</v>
-      </c>
-      <c r="F5" s="55" t="s">
-        <v>186</v>
-      </c>
-      <c r="G5" s="55" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="52" t="s">
-        <v>240</v>
-      </c>
-      <c r="B6" s="53" t="s">
-        <v>146</v>
-      </c>
-      <c r="C6" s="52" t="s">
+      <c r="B13" s="46" t="s">
+        <v>150</v>
+      </c>
+      <c r="C13" s="45" t="s">
+        <v>155</v>
+      </c>
+      <c r="D13" s="46" t="s">
+        <v>151</v>
+      </c>
+      <c r="E13" s="47" t="s">
+        <v>209</v>
+      </c>
+      <c r="F13" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="G13" s="48" t="s">
         <v>154</v>
       </c>
-      <c r="D6" s="53" t="s">
-        <v>144</v>
-      </c>
-      <c r="E6" s="54" t="s">
-        <v>183</v>
-      </c>
-      <c r="F6" s="55" t="s">
-        <v>186</v>
-      </c>
-      <c r="G6" s="55" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="52" t="s">
-        <v>242</v>
-      </c>
-      <c r="B7" s="53" t="s">
-        <v>148</v>
-      </c>
-      <c r="C7" s="52" t="s">
-        <v>154</v>
-      </c>
-      <c r="D7" s="53" t="s">
-        <v>144</v>
-      </c>
-      <c r="E7" s="54" t="s">
-        <v>183</v>
-      </c>
-      <c r="F7" s="55" t="s">
-        <v>186</v>
-      </c>
-      <c r="G7" s="55" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="52" t="s">
-        <v>243</v>
-      </c>
-      <c r="B8" s="53" t="s">
-        <v>142</v>
-      </c>
-      <c r="C8" s="52" t="s">
-        <v>156</v>
-      </c>
-      <c r="D8" s="53" t="s">
-        <v>144</v>
-      </c>
-      <c r="E8" s="54" t="s">
-        <v>183</v>
-      </c>
-      <c r="F8" s="55" t="s">
-        <v>186</v>
-      </c>
-      <c r="G8" s="55" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A9" s="52" t="s">
-        <v>244</v>
-      </c>
-      <c r="B9" s="53" t="s">
-        <v>146</v>
-      </c>
-      <c r="C9" s="52" t="s">
-        <v>156</v>
-      </c>
-      <c r="D9" s="53" t="s">
-        <v>144</v>
-      </c>
-      <c r="E9" s="54" t="s">
-        <v>183</v>
-      </c>
-      <c r="F9" s="55" t="s">
-        <v>186</v>
-      </c>
-      <c r="G9" s="55" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="52" t="s">
-        <v>241</v>
-      </c>
-      <c r="B10" s="53" t="s">
-        <v>148</v>
-      </c>
-      <c r="C10" s="52" t="s">
-        <v>156</v>
-      </c>
-      <c r="D10" s="53" t="s">
-        <v>144</v>
-      </c>
-      <c r="E10" s="54" t="s">
-        <v>183</v>
-      </c>
-      <c r="F10" s="55" t="s">
-        <v>186</v>
-      </c>
-      <c r="G10" s="55" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="52" t="s">
-        <v>150</v>
-      </c>
-      <c r="B11" s="53" t="s">
-        <v>151</v>
-      </c>
-      <c r="C11" s="52" t="s">
-        <v>143</v>
-      </c>
-      <c r="D11" s="53" t="s">
-        <v>152</v>
-      </c>
-      <c r="E11" s="54" t="s">
+    </row>
+    <row r="14" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A14" s="45" t="s">
+        <v>208</v>
+      </c>
+      <c r="B14" s="46"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="47" t="s">
+        <v>211</v>
+      </c>
+      <c r="F14" s="48" t="s">
         <v>210</v>
       </c>
-      <c r="F11" s="55" t="s">
-        <v>186</v>
-      </c>
-      <c r="G11" s="55" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="52" t="s">
-        <v>153</v>
-      </c>
-      <c r="B12" s="53" t="s">
-        <v>151</v>
-      </c>
-      <c r="C12" s="52" t="s">
-        <v>154</v>
-      </c>
-      <c r="D12" s="53" t="s">
-        <v>152</v>
-      </c>
-      <c r="E12" s="54" t="s">
-        <v>210</v>
-      </c>
-      <c r="F12" s="55" t="s">
-        <v>186</v>
-      </c>
-      <c r="G12" s="55" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A13" s="52" t="s">
-        <v>155</v>
-      </c>
-      <c r="B13" s="53" t="s">
-        <v>151</v>
-      </c>
-      <c r="C13" s="52" t="s">
-        <v>156</v>
-      </c>
-      <c r="D13" s="53" t="s">
-        <v>152</v>
-      </c>
-      <c r="E13" s="54" t="s">
-        <v>210</v>
-      </c>
-      <c r="F13" s="55" t="s">
-        <v>186</v>
-      </c>
-      <c r="G13" s="55" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="52" t="s">
-        <v>209</v>
-      </c>
-      <c r="B14" s="53"/>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="54" t="s">
-        <v>212</v>
-      </c>
-      <c r="F14" s="55" t="s">
-        <v>211</v>
-      </c>
-      <c r="G14" s="52"/>
+      <c r="G14" s="45"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="41"/>
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="G15" s="41"/>
+      <c r="A15" s="34"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="G15" s="34"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E16" s="41"/>
+      <c r="E16" s="34"/>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E17" s="41"/>
+      <c r="E17" s="34"/>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E18" s="41"/>
+      <c r="E18" s="34"/>
     </row>
     <row r="19" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E19" s="41"/>
+      <c r="E19" s="34"/>
     </row>
     <row r="20" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E20" s="41"/>
+      <c r="E20" s="34"/>
     </row>
     <row r="21" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E21" s="41"/>
+      <c r="E21" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3975,50 +3974,50 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="41"/>
-      <c r="B1" s="41" t="s">
-        <v>170</v>
-      </c>
-      <c r="C1" s="41" t="s">
-        <v>198</v>
-      </c>
-      <c r="D1" s="41"/>
+      <c r="A1" s="34"/>
+      <c r="B1" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>197</v>
+      </c>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" s="34"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="34" t="s">
         <v>201</v>
       </c>
-      <c r="B2" s="45" t="s">
-        <v>157</v>
-      </c>
-      <c r="C2" s="41" t="s">
+      <c r="B3" s="38" t="s">
         <v>158</v>
       </c>
-      <c r="D2" s="41"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="41" t="s">
-        <v>202</v>
-      </c>
-      <c r="B3" s="45" t="s">
+      <c r="C3" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="C3" s="41" t="s">
-        <v>160</v>
-      </c>
-      <c r="D3" s="41"/>
+      <c r="D3" s="34"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="41"/>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="41"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4030,145 +4029,146 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>193</v>
-      </c>
       <c r="D1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="B2" s="44" t="s">
-        <v>191</v>
+        <v>188</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>190</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="D2" s="48" t="s">
-        <v>179</v>
+        <v>193</v>
+      </c>
+      <c r="D2" s="41" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="B3" s="44" t="s">
-        <v>196</v>
+        <v>189</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>195</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="D3" s="48" t="s">
-        <v>179</v>
+        <v>194</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>246</v>
+      </c>
+      <c r="C4" s="34" t="s">
         <v>218</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="D4" s="41" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="34" t="s">
+        <v>219</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>248</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="34" t="s">
+        <v>220</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>249</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>247</v>
+      </c>
+      <c r="D6" s="41" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="34" t="s">
+        <v>221</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>250</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="D7" s="41" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="34" t="s">
+        <v>222</v>
+      </c>
+      <c r="B8" s="37" t="s">
+        <v>228</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="D8" s="41" t="s">
         <v>230</v>
       </c>
-      <c r="C4" s="41" t="s">
-        <v>219</v>
-      </c>
-      <c r="D4" s="48" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="41" t="s">
-        <v>220</v>
-      </c>
-      <c r="B5" s="44" t="s">
-        <v>231</v>
-      </c>
-      <c r="C5" s="41" t="s">
-        <v>225</v>
-      </c>
-      <c r="D5" s="48" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="41" t="s">
-        <v>221</v>
-      </c>
-      <c r="B6" s="44" t="s">
-        <v>232</v>
-      </c>
-      <c r="C6" s="41" t="s">
-        <v>226</v>
-      </c>
-      <c r="D6" s="48" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="41" t="s">
-        <v>222</v>
-      </c>
-      <c r="B7" s="44" t="s">
-        <v>233</v>
-      </c>
-      <c r="C7" s="41" t="s">
+    </row>
+    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="34" t="s">
+        <v>223</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="C9" s="34" t="s">
         <v>227</v>
       </c>
-      <c r="D7" s="48" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="41" t="s">
-        <v>223</v>
-      </c>
-      <c r="B8" s="44" t="s">
-        <v>234</v>
-      </c>
-      <c r="C8" s="41" t="s">
-        <v>228</v>
-      </c>
-      <c r="D8" s="48" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="41" t="s">
-        <v>224</v>
-      </c>
-      <c r="B9" s="44" t="s">
-        <v>235</v>
-      </c>
-      <c r="C9" s="41" t="s">
-        <v>229</v>
-      </c>
-      <c r="D9" s="48" t="s">
-        <v>236</v>
+      <c r="D9" s="41" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="41"/>
-      <c r="B10" s="44"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="37"/>
     </row>
     <row r="24" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G24" s="41"/>
+      <c r="G24" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changes for national competitions
</commit_message>
<xml_diff>
--- a/media/comp_data_2018.xlsx
+++ b/media/comp_data_2018.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="competitions" sheetId="26" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="279">
   <si>
     <t>PP</t>
   </si>
@@ -798,13 +798,91 @@
   </si>
   <si>
     <t>விசேட முன்னேற்பாடற்ற பேச்சுப் போட்டி -  அதிஇளைஞர் பிரிவு</t>
+  </si>
+  <si>
+    <t>First Prize (Gold Medal)</t>
+  </si>
+  <si>
+    <t>Kjy; (jq;fg;gjf;fk;)</t>
+  </si>
+  <si>
+    <t>National</t>
+  </si>
+  <si>
+    <t>at the</t>
+  </si>
+  <si>
+    <t>National level.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Njrpaepiyapy; eilngw;w  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">khepy epiyapy; eilngw;w </t>
+  </si>
+  <si>
+    <t>,uz;lhk; (nts;spg;gjf;fk;)</t>
+  </si>
+  <si>
+    <t>%d;whk; (ntz;fyg;gjf;fk;)</t>
+  </si>
+  <si>
+    <t>Second Prize (Silver Medal)</t>
+  </si>
+  <si>
+    <t>Third Prize (Bronze Medal)</t>
+  </si>
+  <si>
+    <t>Fourth Prize</t>
+  </si>
+  <si>
+    <t>Fifth Prize</t>
+  </si>
+  <si>
+    <t>Sixth Prize</t>
+  </si>
+  <si>
+    <t>Seventh Prize</t>
+  </si>
+  <si>
+    <t>Eighth Prize</t>
+  </si>
+  <si>
+    <t>Tenth Prize</t>
+  </si>
+  <si>
+    <t>ehd;fhk;</t>
+  </si>
+  <si>
+    <t>Mwhk;</t>
+  </si>
+  <si>
+    <t>Ie;jhk;</t>
+  </si>
+  <si>
+    <t>Vohk;</t>
+  </si>
+  <si>
+    <t>vl;lhk;</t>
+  </si>
+  <si>
+    <t>Ninth Prize</t>
+  </si>
+  <si>
+    <t>xd;gjhk;</t>
+  </si>
+  <si>
+    <t>gj;jhk;</t>
+  </si>
+  <si>
+    <t>Pending</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -944,6 +1022,16 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Bamini Plain"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1093,11 +1181,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1224,10 +1313,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1529,7 +1623,7 @@
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -3297,7 +3391,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3604,16 +3698,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" customWidth="1"/>
     <col min="5" max="5" width="46.1640625" style="33" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34.83203125" style="34" customWidth="1"/>
@@ -3932,31 +4026,190 @@
       </c>
       <c r="G14" s="45"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="34"/>
-      <c r="B15" s="34"/>
+    <row r="15" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="45" t="s">
+        <v>253</v>
+      </c>
+      <c r="B15" s="53" t="s">
+        <v>254</v>
+      </c>
       <c r="C15" s="34"/>
       <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="G15" s="34"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E16" s="34"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E17" s="34"/>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E18" s="34"/>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E19" s="34"/>
-    </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E20" s="34"/>
-    </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E21" s="34"/>
+      <c r="E15" s="47" t="s">
+        <v>209</v>
+      </c>
+      <c r="F15" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="G15" s="48" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A16" s="45" t="s">
+        <v>262</v>
+      </c>
+      <c r="B16" s="55" t="s">
+        <v>260</v>
+      </c>
+      <c r="C16" s="45"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="47" t="s">
+        <v>209</v>
+      </c>
+      <c r="F16" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="G16" s="48" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A17" s="45" t="s">
+        <v>263</v>
+      </c>
+      <c r="B17" s="55" t="s">
+        <v>261</v>
+      </c>
+      <c r="C17" s="45"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="47" t="s">
+        <v>209</v>
+      </c>
+      <c r="F17" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="G17" s="48" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="21" x14ac:dyDescent="0.2">
+      <c r="A18" s="52" t="s">
+        <v>264</v>
+      </c>
+      <c r="B18" s="55" t="s">
+        <v>270</v>
+      </c>
+      <c r="E18" s="47" t="s">
+        <v>209</v>
+      </c>
+      <c r="F18" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="G18" s="48" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A19" s="45" t="s">
+        <v>265</v>
+      </c>
+      <c r="B19" s="55" t="s">
+        <v>272</v>
+      </c>
+      <c r="E19" s="47" t="s">
+        <v>209</v>
+      </c>
+      <c r="F19" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="G19" s="48" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A20" s="45" t="s">
+        <v>266</v>
+      </c>
+      <c r="B20" s="55" t="s">
+        <v>271</v>
+      </c>
+      <c r="E20" s="47" t="s">
+        <v>209</v>
+      </c>
+      <c r="F20" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="G20" s="48" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A21" s="45" t="s">
+        <v>267</v>
+      </c>
+      <c r="B21" s="55" t="s">
+        <v>273</v>
+      </c>
+      <c r="E21" s="47" t="s">
+        <v>209</v>
+      </c>
+      <c r="F21" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="G21" s="48" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A22" s="45" t="s">
+        <v>268</v>
+      </c>
+      <c r="B22" s="55" t="s">
+        <v>274</v>
+      </c>
+      <c r="E22" s="47" t="s">
+        <v>209</v>
+      </c>
+      <c r="F22" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="G22" s="48" t="s">
+        <v>268</v>
+      </c>
+      <c r="I22" s="53"/>
+    </row>
+    <row r="23" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A23" s="45" t="s">
+        <v>275</v>
+      </c>
+      <c r="B23" s="55" t="s">
+        <v>276</v>
+      </c>
+      <c r="E23" s="47" t="s">
+        <v>209</v>
+      </c>
+      <c r="F23" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="G23" s="48" t="s">
+        <v>275</v>
+      </c>
+      <c r="I23" s="53"/>
+    </row>
+    <row r="24" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A24" s="45" t="s">
+        <v>269</v>
+      </c>
+      <c r="B24" s="55" t="s">
+        <v>277</v>
+      </c>
+      <c r="E24" s="47" t="s">
+        <v>209</v>
+      </c>
+      <c r="F24" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="G24" s="48" t="s">
+        <v>269</v>
+      </c>
+      <c r="I24" s="53"/>
+    </row>
+    <row r="25" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A25" s="45" t="s">
+        <v>278</v>
+      </c>
+      <c r="I25" s="53"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4026,149 +4279,188 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
         <v>191</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>188</v>
       </c>
       <c r="B2" s="37" t="s">
         <v>190</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="37" t="s">
+        <v>259</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="E2" s="41" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>189</v>
       </c>
       <c r="B3" s="37" t="s">
         <v>195</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="37" t="s">
+        <v>259</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="E3" s="41" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>217</v>
       </c>
       <c r="B4" s="37" t="s">
         <v>246</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="37" t="s">
+        <v>259</v>
+      </c>
+      <c r="D4" s="34" t="s">
         <v>218</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="E4" s="41" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="34" t="s">
         <v>219</v>
       </c>
       <c r="B5" s="37" t="s">
         <v>248</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="37" t="s">
+        <v>259</v>
+      </c>
+      <c r="D5" s="34" t="s">
         <v>224</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="E5" s="41" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="34" t="s">
         <v>220</v>
       </c>
       <c r="B6" s="37" t="s">
         <v>249</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="37" t="s">
+        <v>259</v>
+      </c>
+      <c r="D6" s="34" t="s">
         <v>247</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="E6" s="41" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="34" t="s">
         <v>221</v>
       </c>
       <c r="B7" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="37" t="s">
+        <v>259</v>
+      </c>
+      <c r="D7" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="E7" s="41" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="34" t="s">
         <v>222</v>
       </c>
       <c r="B8" s="37" t="s">
         <v>228</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="37" t="s">
+        <v>259</v>
+      </c>
+      <c r="D8" s="34" t="s">
         <v>226</v>
       </c>
-      <c r="D8" s="41" t="s">
+      <c r="E8" s="41" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="34" t="s">
         <v>223</v>
       </c>
       <c r="B9" s="37" t="s">
         <v>229</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="37" t="s">
+        <v>259</v>
+      </c>
+      <c r="D9" s="34" t="s">
         <v>227</v>
       </c>
-      <c r="D9" s="41" t="s">
+      <c r="E9" s="41" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="34"/>
-      <c r="B10" s="37"/>
-    </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G24" s="34"/>
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="41" t="s">
+        <v>255</v>
+      </c>
+      <c r="B10" s="41"/>
+      <c r="C10" s="54" t="s">
+        <v>258</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>256</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="24" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H24" s="54"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>